<commit_message>
reorganize common mistakes and add screenshots
</commit_message>
<xml_diff>
--- a/data/SAFI_examples.xlsx
+++ b/data/SAFI_examples.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11440" yWindow="800" windowWidth="21740" windowHeight="14520"/>
+    <workbookView xWindow="40" yWindow="580" windowWidth="31720" windowHeight="16660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>poultry</t>
   </si>
@@ -66,6 +66,54 @@
   </si>
   <si>
     <t>3, (oxen ,  goats)</t>
+  </si>
+  <si>
+    <t>key_id</t>
+  </si>
+  <si>
+    <t>roof_type</t>
+  </si>
+  <si>
+    <t>wall type</t>
+  </si>
+  <si>
+    <t>floor type</t>
+  </si>
+  <si>
+    <t>rooms</t>
+  </si>
+  <si>
+    <t>grass</t>
+  </si>
+  <si>
+    <t>muddaub</t>
+  </si>
+  <si>
+    <t>errth</t>
+  </si>
+  <si>
+    <t>earth</t>
+  </si>
+  <si>
+    <t>mabati_sloping</t>
+  </si>
+  <si>
+    <t>burntbricks</t>
+  </si>
+  <si>
+    <t>cement</t>
+  </si>
+  <si>
+    <t>mabatisloping</t>
+  </si>
+  <si>
+    <t>inc_barn</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -403,7 +451,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -546,6 +594,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -591,12 +648,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -952,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:H14"/>
+  <dimension ref="C5:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -963,9 +1026,15 @@
     <col min="3" max="3" width="48" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="25.1640625" customWidth="1"/>
+    <col min="12" max="12" width="18.83203125" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:15" ht="26" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
@@ -981,8 +1050,13 @@
       <c r="H5" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="3:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:15" ht="26" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
@@ -998,8 +1072,26 @@
       <c r="H6" s="3">
         <v>0</v>
       </c>
+      <c r="J6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="7" spans="3:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:15" ht="26" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1015,8 +1107,26 @@
       <c r="H7" s="3">
         <v>1</v>
       </c>
+      <c r="J7" s="5">
+        <v>1</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="5">
+        <v>1</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="8" spans="3:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:15" ht="26" x14ac:dyDescent="0.3">
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1032,8 +1142,26 @@
       <c r="H8" s="3">
         <v>0</v>
       </c>
+      <c r="J8" s="5">
+        <v>2</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="5">
+        <v>1</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="9" spans="3:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:15" ht="26" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1049,8 +1177,26 @@
       <c r="H9" s="3">
         <v>1</v>
       </c>
+      <c r="J9" s="5">
+        <v>3</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="5">
+        <v>-99</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="10" spans="3:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:15" ht="26" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1066,8 +1212,26 @@
       <c r="H10" s="3">
         <v>1</v>
       </c>
+      <c r="J10" s="5">
+        <v>4</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="5">
+        <v>1</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="11" spans="3:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:15" ht="26" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1083,8 +1247,26 @@
       <c r="H11" s="3">
         <v>0</v>
       </c>
+      <c r="J11" s="5">
+        <v>5</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="5">
+        <v>1</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="12" spans="3:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:15" ht="26" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
         <v>1</v>
       </c>
@@ -1100,8 +1282,26 @@
       <c r="H12" s="3">
         <v>1</v>
       </c>
+      <c r="J12" s="5">
+        <v>6</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N12" s="5">
+        <v>1</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="13" spans="3:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:15" ht="26" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1117,8 +1317,26 @@
       <c r="H13" s="3">
         <v>1</v>
       </c>
+      <c r="J13" s="5">
+        <v>7</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="5">
+        <v>1</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="14" spans="3:8" ht="26" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:15" ht="26" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1134,8 +1352,69 @@
       <c r="H14" s="3">
         <v>1</v>
       </c>
+      <c r="J14" s="5">
+        <v>8</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" s="5">
+        <v>3</v>
+      </c>
+      <c r="O14" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" ht="26" x14ac:dyDescent="0.3">
+      <c r="J15" s="5">
+        <v>9</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" s="5">
+        <v>1</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" ht="26" x14ac:dyDescent="0.3">
+      <c r="J16" s="5">
+        <v>10</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N16" s="5">
+        <v>5</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K5:N5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>